<commit_message>
JCSantos - Casi OK
</commit_message>
<xml_diff>
--- a/Extra/libros_flumperio@gmail.com.xlsx
+++ b/Extra/libros_flumperio@gmail.com.xlsx
@@ -26,16 +26,16 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-                        Conservación y restauración de materiales metálicos
+                        CARA A CARA CON SATANÁS
                     </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">
-                        Barrio Martín, Joaquín / Medina Sánchez, María Cruz / Cabello Briones, Cristina / Pardo Naranjo, Ana Isabel / Donate Carretero, Inmaculada / Serrano Moreno, Juan
+                        PORQUERAS, TERESA
                                             </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">978-84-1357-141-6 </x:t>
+    <x:t xml:space="preserve">978-84-122549-4-5 </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">

</xml_diff>